<commit_message>
added FTDI chip to bom
</commit_message>
<xml_diff>
--- a/BOM/BOM_4-24.xlsx
+++ b/BOM/BOM_4-24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chase\Documents\KiCAD\Senior_Design\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F497BF91-73CE-428C-8A47-E85ED9CD147A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C52D2D-180D-4FCC-A6D1-7817531A8F8A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{EF5B7B3E-C4F0-45DA-ACF0-EF0C51E326DB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="130">
   <si>
     <t>Type</t>
   </si>
@@ -403,6 +403,18 @@
   </si>
   <si>
     <t>Poly-fuse</t>
+  </si>
+  <si>
+    <t>USB-Serial</t>
+  </si>
+  <si>
+    <t>FT231XS-R</t>
+  </si>
+  <si>
+    <t>SSOP-20</t>
+  </si>
+  <si>
+    <t>2.12</t>
   </si>
 </sst>
 </file>
@@ -510,8 +522,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{798CF35B-6132-43C7-8F9B-3E504A3745E2}" name="Table1" displayName="Table1" ref="A2:I44" totalsRowCount="1">
-  <autoFilter ref="A2:I43" xr:uid="{1BDD39F1-B251-46F9-8166-33FBFC737F37}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{798CF35B-6132-43C7-8F9B-3E504A3745E2}" name="Table1" displayName="Table1" ref="A2:I45" totalsRowCount="1">
+  <autoFilter ref="A2:I44" xr:uid="{1BDD39F1-B251-46F9-8166-33FBFC737F37}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2A3D66EE-0ABB-433B-9F39-B598B17029C8}" name="#"/>
     <tableColumn id="2" xr3:uid="{EC282E2A-6E44-40D2-9DB6-24970CE2C145}" name="Type"/>
@@ -828,10 +840,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E7DFE5-1BAC-4EDF-9D8B-8E92D715E45B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,27 +2003,26 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>37</v>
+        <v>126</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E42" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G42">
-        <v>0.24</v>
-      </c>
-      <c r="H42" s="3"/>
-      <c r="I42">
-        <f>Table1[[#This Row],['#]]*Table1[[#This Row],[price]]</f>
-        <v>0.24</v>
+        <v>128</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I42" s="2">
+        <f>Table1[[#This Row],['#]]*Table1[[#This Row],[price]]</f>
+        <v>2.12</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2019,39 +2030,67 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43" t="s">
+        <v>111</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G43">
+        <v>0.24</v>
+      </c>
+      <c r="H43" s="3"/>
+      <c r="I43">
+        <f>Table1[[#This Row],['#]]*Table1[[#This Row],[price]]</f>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
         <v>38</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>39</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>113</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="G43">
+      <c r="G44">
         <v>0.72</v>
       </c>
-      <c r="H43" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I43">
+      <c r="H44" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I44">
         <f>Table1[[#This Row],['#]]*Table1[[#This Row],[price]]</f>
         <v>0.72</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G44" s="3"/>
-      <c r="H44" s="3" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G45" s="3"/>
+      <c r="H45" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I45" s="2">
         <f>SUM(Table1[Total])</f>
-        <v>65.589999999999989</v>
+        <v>67.709999999999994</v>
       </c>
     </row>
   </sheetData>
@@ -2097,13 +2136,14 @@
     <hyperlink ref="D37" r:id="rId33" display="https://www.mouser.com/ProductDetail/Microchip-Technology/AT42QT1010-MAH?qs=sGAEpiMZZMv%2fbGM7XKYHK%252b0NDZ2i1W%252bX" xr:uid="{11BA334C-4BAB-416E-96D8-E0CA36923B34}"/>
     <hyperlink ref="D40" r:id="rId34" display="https://www.mouser.com/ProductDetail/Texas-Instruments/LM358ADR?qs=sGAEpiMZZMtYFXwiBRPs0zFXHJUd7gdT" xr:uid="{2DADAC72-F982-4292-AF89-255A95AF9B77}"/>
     <hyperlink ref="D41" r:id="rId35" display="https://www.mouser.com/ProductDetail/Texas-Instruments/INA169NA-3K?qs=sGAEpiMZZMuo%252bmZx5g6tFD8TTXQDX2ot" xr:uid="{30EE367D-EDE1-4175-A6BA-F6A77EB7BEFB}"/>
-    <hyperlink ref="D42" r:id="rId36" display="https://www.mouser.com/ProductDetail/IQD/LFXTAL033808Reel?qs=sGAEpiMZZMsBj6bBr9Q9af1kE%252bXo19x3D66o2Mb0OuifZBqfW0Zkgw%3d%3d" xr:uid="{2AACB80A-20B1-431A-B3D7-EB4B0F352B17}"/>
-    <hyperlink ref="D43" r:id="rId37" display="https://www.mouser.com/ProductDetail/TDK/PS1240P02BT?qs=sGAEpiMZZMs%252b6Ea5iKw4JnKB8rEmL0Rz" xr:uid="{282A3AE2-CE80-4BF6-9AE9-A7640C422DD3}"/>
+    <hyperlink ref="D43" r:id="rId36" display="https://www.mouser.com/ProductDetail/IQD/LFXTAL033808Reel?qs=sGAEpiMZZMsBj6bBr9Q9af1kE%252bXo19x3D66o2Mb0OuifZBqfW0Zkgw%3d%3d" xr:uid="{2AACB80A-20B1-431A-B3D7-EB4B0F352B17}"/>
+    <hyperlink ref="D44" r:id="rId37" display="https://www.mouser.com/ProductDetail/TDK/PS1240P02BT?qs=sGAEpiMZZMs%252b6Ea5iKw4JnKB8rEmL0Rz" xr:uid="{282A3AE2-CE80-4BF6-9AE9-A7640C422DD3}"/>
+    <hyperlink ref="D42" r:id="rId38" display="https://www.mouser.com/ProductDetail/FTDI/FT231XS-R?qs=sGAEpiMZZMvVkErl6zY%252bqfBUiQa5NfR7" xr:uid="{F8BB2A2F-19CF-4DF9-9774-3CDB418EA220}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId38"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
   <tableParts count="1">
-    <tablePart r:id="rId39"/>
+    <tablePart r:id="rId40"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
99 percent ready to order
</commit_message>
<xml_diff>
--- a/BOM/BOM_4-24.xlsx
+++ b/BOM/BOM_4-24.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chase\Documents\KiCAD\Senior_Design\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C52D2D-180D-4FCC-A6D1-7817531A8F8A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEFFC20-CC37-49DC-B455-65B957A956D7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{EF5B7B3E-C4F0-45DA-ACF0-EF0C51E326DB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="142">
   <si>
     <t>Type</t>
   </si>
@@ -415,13 +415,49 @@
   </si>
   <si>
     <t>2.12</t>
+  </si>
+  <si>
+    <t>REF</t>
+  </si>
+  <si>
+    <t>QTY per Brd</t>
+  </si>
+  <si>
+    <t>footprint check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C102 C103 C109 C110 C202 C203 C302 C305 C501 C502 C602 C603 </t>
+  </si>
+  <si>
+    <t>NOTES2</t>
+  </si>
+  <si>
+    <t>NEEDS 12 PER BOARD, NOT FOR ORDER (&gt;12</t>
+  </si>
+  <si>
+    <t>missing components</t>
+  </si>
+  <si>
+    <t>two types of 100k on BOM</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>~4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R104 R105 R202 R602   </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -451,13 +487,39 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -473,7 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -484,6 +546,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -500,10 +571,10 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -522,21 +593,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{798CF35B-6132-43C7-8F9B-3E504A3745E2}" name="Table1" displayName="Table1" ref="A2:I45" totalsRowCount="1">
-  <autoFilter ref="A2:I44" xr:uid="{1BDD39F1-B251-46F9-8166-33FBFC737F37}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{798CF35B-6132-43C7-8F9B-3E504A3745E2}" name="Table1" displayName="Table1" ref="A2:M45" totalsRowCount="1">
+  <autoFilter ref="A2:M44" xr:uid="{1BDD39F1-B251-46F9-8166-33FBFC737F37}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{2A3D66EE-0ABB-433B-9F39-B598B17029C8}" name="#"/>
     <tableColumn id="2" xr3:uid="{EC282E2A-6E44-40D2-9DB6-24970CE2C145}" name="Type"/>
     <tableColumn id="3" xr3:uid="{1D35EB73-661E-48D5-BC3D-74AA70CC7CEC}" name="Value"/>
     <tableColumn id="4" xr3:uid="{C48B5B29-F2A4-4F9A-B6D6-822A0463AE79}" name="PN"/>
     <tableColumn id="5" xr3:uid="{725101C0-98AA-4B54-B988-4DB0BA617EE5}" name="Notes"/>
     <tableColumn id="6" xr3:uid="{869CA174-13FD-4385-9FB8-06CEBB9ADD74}" name="footprint"/>
-    <tableColumn id="7" xr3:uid="{F3CCE7B5-30DA-406F-AE08-9E2078A55EC5}" name="price" dataDxfId="5" totalsRowDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{4B00B9D6-4228-4FB7-9F7E-46D0C798CC6E}" name="Dist." totalsRowLabel="Total " dataDxfId="4" totalsRowDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{CC731685-C35F-44DB-8E59-F8501C7A4408}" name="Total" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="0">
+    <tableColumn id="7" xr3:uid="{F3CCE7B5-30DA-406F-AE08-9E2078A55EC5}" name="price" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{4B00B9D6-4228-4FB7-9F7E-46D0C798CC6E}" name="Dist." totalsRowLabel="Total " dataDxfId="5" totalsRowDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{CC731685-C35F-44DB-8E59-F8501C7A4408}" name="Total" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],['#]]*Table1[[#This Row],[price]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table1[Total])</totalsRowFormula>
     </tableColumn>
+    <tableColumn id="8" xr3:uid="{E37817B6-CC50-47A7-9D18-CC01E23AC561}" name="REF"/>
+    <tableColumn id="11" xr3:uid="{B9DE72FC-DB87-44E1-B834-99F12753A6EC}" name="QTY per Brd"/>
+    <tableColumn id="12" xr3:uid="{9A61E970-078C-4978-9E75-2646100B7598}" name="footprint check"/>
+    <tableColumn id="13" xr3:uid="{FA8928F0-17DA-4D37-914F-B85963929889}" name="NOTES2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -840,10 +915,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E7DFE5-1BAC-4EDF-9D8B-8E92D715E45B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,14 +927,17 @@
     <col min="2" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>40</v>
       </c>
@@ -871,15 +949,18 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>118</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
@@ -888,7 +969,7 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="11" t="s">
         <v>44</v>
       </c>
       <c r="G2" t="s">
@@ -900,8 +981,20 @@
       <c r="I2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -931,7 +1024,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -961,7 +1054,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -991,7 +1084,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>25</v>
       </c>
@@ -1021,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1051,37 +1144,49 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="10">
         <v>0.18</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I8">
+      <c r="H8" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="10">
         <f>Table1[[#This Row],['#]]*Table1[[#This Row],[price]]</f>
         <v>2.16</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="K8" s="10">
+        <v>12</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="M8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12</v>
       </c>
@@ -1111,7 +1216,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1138,7 +1243,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1165,7 +1270,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1192,7 +1297,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1216,7 +1321,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1246,7 +1351,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1276,7 +1381,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1303,7 +1408,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1333,7 +1438,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1363,7 +1468,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1393,7 +1498,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1423,7 +1528,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1450,7 +1555,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1477,7 +1582,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1504,7 +1609,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>14</v>
       </c>
@@ -1534,7 +1639,7 @@
         <v>1.4000000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1561,7 +1666,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1588,7 +1693,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20</v>
       </c>
@@ -1618,7 +1723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1645,7 +1750,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1672,34 +1777,47 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
         <v>10</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I30">
+      <c r="G30" s="8"/>
+      <c r="H30" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I30" s="8">
         <f>Table1[[#This Row],['#]]*Table1[[#This Row],[price]]</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>141</v>
+      </c>
+      <c r="K30" t="s">
+        <v>140</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="M30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1729,7 +1847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2</v>
       </c>
@@ -2091,6 +2209,69 @@
       <c r="I45" s="2">
         <f>SUM(Table1[Total])</f>
         <v>67.709999999999994</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A47" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>